<commit_message>
refactoring of data input complete for playoff scheduler
</commit_message>
<xml_diff>
--- a/data input/prelim_data.xlsx
+++ b/data input/prelim_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorprieto/Desktop/code/cornerstone/inputs/master_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorprieto/Desktop/code/cornerstone/data input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75D3B98-2F97-9341-91D3-08494279E608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C07351-E550-F445-97BD-8A3C9EE21942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{2114AE23-4723-3F48-88AE-F53CC59B0CBE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="130">
   <si>
     <t>Team</t>
   </si>
@@ -366,9 +366,6 @@
     <t>Enter tournament date here.</t>
   </si>
   <si>
-    <t>Enter "Y" or "N" for QR codes to be included.</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -411,10 +408,25 @@
     <t>Individualized Room Prelim Schedule</t>
   </si>
   <si>
-    <t>Enter "Y" or "N" for text input to be included.</t>
-  </si>
-  <si>
     <t>Prelim Group Names</t>
+  </si>
+  <si>
+    <t>This is the placeholder text for the prelim schedule individualized for each team. Useful pieces of information to include in this section are: expected start time and length of time for lunch, information on tiebreakers, where to report back after lunch...</t>
+  </si>
+  <si>
+    <t>This is the placeholder text for the prelim schedule individualized for each room. Useful pieces of information to include in this section are: how to report protests, tiebreaker procedure, where to go for lunch…</t>
+  </si>
+  <si>
+    <t>Enter "Y" for QR codes to be included or "N" to be excluded.</t>
+  </si>
+  <si>
+    <t>Enter "Y" for text input to be included or "N" to be excluded.</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -592,7 +604,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -633,6 +645,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -954,7 +972,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
@@ -980,7 +998,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>106</v>
@@ -991,7 +1009,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>107</v>
@@ -1013,54 +1031,54 @@
         <v>104</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="11" t="s">
         <v>109</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>124</v>
+        <v>129</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="5">
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="5">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="5">
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1085,7 +1103,7 @@
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
@@ -1571,9 +1589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF3F05E-06AC-6A4B-A200-208805A45293}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView zoomScale="267" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="267" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
@@ -1582,7 +1598,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="2" customFormat="1" ht="40" customHeight="1">
@@ -1643,9 +1659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B02CA44-6EE3-1E45-A0FA-E7B275D443B3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="184" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView zoomScale="184" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
@@ -1856,9 +1870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10058E87-174A-E14F-9AEE-7ACFACE9B5BB}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="184" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView zoomScale="184" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
@@ -1870,16 +1882,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1887,7 +1899,7 @@
         <v>86</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>93</v>
@@ -1901,7 +1913,7 @@
         <v>87</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>94</v>
@@ -1915,7 +1927,7 @@
         <v>88</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>95</v>
@@ -1929,7 +1941,7 @@
         <v>89</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>96</v>
@@ -1943,7 +1955,7 @@
         <v>90</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>97</v>
@@ -1957,7 +1969,7 @@
         <v>91</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>98</v>
@@ -1977,9 +1989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3F142A-4698-834F-8261-DB2006E5DBFB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="184" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView zoomScale="184" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
@@ -1987,30 +1997,28 @@
     <col min="2" max="2" width="47.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="40" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    </row>
+    <row r="2" spans="1:2" ht="160" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="160" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="10" t="str">
-        <f>"Text to insert in "&amp;A2</f>
-        <v>Text to insert in Individualized Team Prelim Schedule</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="10" t="str">
-        <f t="shared" ref="B3" si="0">"Text to insert in "&amp;A3</f>
-        <v>Text to insert in Individualized Room Prelim Schedule</v>
+      <c r="B3" s="15" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>